<commit_message>
actualización del flujo de caja
Se agregaron los nuevos valores del flujo de caja
</commit_message>
<xml_diff>
--- a/Fase 2/documentacion/Documentos Grupales/FLUJO DE CAJA.xlsx
+++ b/Fase 2/documentacion/Documentos Grupales/FLUJO DE CAJA.xlsx
@@ -9,16 +9,16 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FoTBwVVHpV0Lc3WEq6F03W/gH5CUTadbPD76QAekoSM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="zgJM81/ilW1fBT3JAhRgPTqaqraDj6M2VdWnfNclJ0o="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
-  <si>
-    <t xml:space="preserve">ITEM </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="33">
+  <si>
+    <t>ITEM</t>
   </si>
   <si>
     <t>MES 0</t>
@@ -27,160 +27,106 @@
     <t>AGOSTO</t>
   </si>
   <si>
-    <t xml:space="preserve">SEPTIEMBRE </t>
+    <t>SEPTIEMBRE</t>
   </si>
   <si>
     <t>OCTUBRE</t>
   </si>
   <si>
-    <t xml:space="preserve">NOVIEMBRE </t>
+    <t>NOVIEMBRE</t>
   </si>
   <si>
     <t>DICIEMBRE</t>
   </si>
   <si>
+    <t>ENERO</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>INGRESO</t>
-  </si>
-  <si>
-    <t>COSTOS INDIRECTOS (DETALLE)</t>
-  </si>
-  <si>
-    <t>Electricidad</t>
-  </si>
-  <si>
-    <t>$ -</t>
-  </si>
-  <si>
-    <t>$   900.000</t>
-  </si>
-  <si>
-    <t>$ 900.000</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>$   600.000</t>
-  </si>
-  <si>
-    <t>$ 600.000</t>
-  </si>
-  <si>
-    <t>Licencias Software</t>
-  </si>
-  <si>
-    <t>$   950.000</t>
-  </si>
-  <si>
-    <t>$ 950.000</t>
-  </si>
-  <si>
-    <t>Uso de Espacio/Hogar</t>
-  </si>
-  <si>
-    <t>$   300.000</t>
-  </si>
-  <si>
-    <t>$ 300.000</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>$   281.277</t>
-  </si>
-  <si>
-    <t>$ 281.277</t>
-  </si>
-  <si>
-    <t>TOTAL COSTOS INDIRECTOS</t>
-  </si>
-  <si>
-    <t>$ 3.031.277</t>
-  </si>
-  <si>
-    <t>Administración y Gestión</t>
-  </si>
-  <si>
-    <t>$ 1.515.638</t>
-  </si>
-  <si>
-    <t>Contingencias y Riesgos</t>
-  </si>
-  <si>
-    <t>$   505.212</t>
-  </si>
-  <si>
-    <t>SUELDOS FASE PLANIFICACION</t>
-  </si>
-  <si>
-    <t>$ 1.667.210</t>
-  </si>
-  <si>
-    <t>SUELDO FASE ANALISIS Y DISEÑO $ -</t>
-  </si>
-  <si>
-    <t>$ 3.820.372</t>
-  </si>
-  <si>
-    <t>$ 7.640.744</t>
-  </si>
-  <si>
-    <t>SUELDO FASE DESARROLLO</t>
-  </si>
-  <si>
-    <t>$ 796.300</t>
-  </si>
-  <si>
-    <t>EGRESOS</t>
-  </si>
-  <si>
-    <t>$ 5.052.127</t>
-  </si>
-  <si>
-    <t>$ 15.156.381</t>
-  </si>
-  <si>
-    <t>FLUJOS</t>
-  </si>
-  <si>
-    <t>-$1.667.210</t>
-  </si>
-  <si>
-    <t>-$3.820.372</t>
-  </si>
-  <si>
-    <t>-$796.300</t>
-  </si>
-  <si>
-    <t>-$5.052.127</t>
-  </si>
-  <si>
-    <t>-$15.156.381</t>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>Préstamo</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Aporte socios</t>
+  </si>
+  <si>
+    <t>Capital semilla</t>
+  </si>
+  <si>
+    <t>Venta Sistema (App+Instalación+Soporte)</t>
+  </si>
+  <si>
+    <t>TOTAL INGRESOS</t>
+  </si>
+  <si>
+    <t>EGRESOS OPERACIONALES</t>
+  </si>
+  <si>
+    <t>Sueldos planificación</t>
+  </si>
+  <si>
+    <t>Sueldos análisis y diseño</t>
+  </si>
+  <si>
+    <t>Sueldo desarrollo</t>
+  </si>
+  <si>
+    <t>Costos indirectos (luz, internet, licencias, etc.)</t>
+  </si>
+  <si>
+    <t>Administración &amp; Gestión</t>
+  </si>
+  <si>
+    <t>Contingencias &amp; Riesgos</t>
+  </si>
+  <si>
+    <t>Subtotal Operacional</t>
+  </si>
+  <si>
+    <t>EGRESOS PRÉSTAMO</t>
+  </si>
+  <si>
+    <t>Pago préstamo cuota 1</t>
+  </si>
+  <si>
+    <t>Pago préstamo cuota 2</t>
+  </si>
+  <si>
+    <t>Pago préstamo cuota 3</t>
+  </si>
+  <si>
+    <t>Pago préstamo cuota 4</t>
+  </si>
+  <si>
+    <t>Subtotal Préstamo</t>
+  </si>
+  <si>
+    <t>TOTAL EGRESOS</t>
+  </si>
+  <si>
+    <t>FLUJO NETO DEL MES</t>
+  </si>
+  <si>
+    <t>SALDO ACUMULADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -203,18 +149,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFBFBFBF"/>
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
-        <bgColor rgb="FF999999"/>
+        <fgColor rgb="FFB7B7B7"/>
+        <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border/>
     <border>
       <left style="thin">
@@ -226,61 +172,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -289,34 +180,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="2" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -534,455 +423,704 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="10.71"/>
-    <col customWidth="1" min="2" max="2" width="28.29"/>
-    <col customWidth="1" min="3" max="3" width="15.29"/>
-    <col customWidth="1" min="4" max="4" width="16.43"/>
-    <col customWidth="1" min="5" max="5" width="15.86"/>
-    <col customWidth="1" min="6" max="6" width="15.14"/>
-    <col customWidth="1" min="7" max="7" width="16.71"/>
-    <col customWidth="1" min="8" max="8" width="18.14"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="15.57"/>
-    <col customWidth="1" min="11" max="21" width="10.71"/>
+    <col customWidth="1" min="2" max="2" width="39.86"/>
+    <col customWidth="1" min="3" max="13" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4">
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8000000.0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4">
+        <v>8000000.0</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7000000.0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7000000.0</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6000000.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4">
+        <v>6000000.0</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2.85E7</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2.85E7</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.1E7</v>
+      </c>
+      <c r="D9" s="5">
         <v>0.0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E9" s="5">
         <v>0.0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F9" s="5">
         <v>0.0</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5">
+      <c r="G9" s="5">
         <v>0.0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H9" s="5">
         <v>0.0</v>
       </c>
-      <c r="I3" s="6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" ref="C4:I4" si="1">SUM(C3)</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="B6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="I9" s="6">
+        <v>2.85E7</v>
+      </c>
+      <c r="J9" s="6">
+        <v>4.95E7</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="12" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1667210.0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1667210.0</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3820372.0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3820372.0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="4">
+        <v>7640744.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.0" customHeight="1">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="12" t="s">
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4">
+        <v>796300.0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4">
+        <v>796300.0</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4">
+        <v>3031277.0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="4">
+        <v>3031277.0</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="C16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1515638.0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1515638.0</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="B10" s="12" t="s">
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4">
+        <v>505212.0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="4">
+        <v>505212.0</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5487582.0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3820372.0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>796300.0</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="6">
+        <v>5052127.0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1.5156381E7</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="B11" s="12" t="s">
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2000000.0</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="4">
+        <v>2000000.0</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="12" t="s">
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2000000.0</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2000000.0</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="B13" s="12" t="s">
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2000000.0</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2000000.0</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="12" t="s">
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2000000.0</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="4">
+        <v>2000000.0</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="B25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" ht="15.0" customHeight="1">
-      <c r="B14" s="12" t="s">
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="6">
+        <v>2000000.0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>2000000.0</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2000000.0</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2000000.0</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="6">
+        <v>8000000.0</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5487582.0</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5820372.0</v>
+      </c>
+      <c r="F27" s="6">
+        <v>2796300.0</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2000000.0</v>
+      </c>
+      <c r="H27" s="6">
+        <v>7052127.0</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2.3156381E7</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="B29" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="B16" s="12" t="s">
+      <c r="C29" s="8">
+        <v>2.1E7</v>
+      </c>
+      <c r="D29" s="8">
+        <v>-5487582.0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>-5820372.0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>-2796300.0</v>
+      </c>
+      <c r="G29" s="8">
+        <v>-2000000.0</v>
+      </c>
+      <c r="H29" s="8">
+        <v>-7052127.0</v>
+      </c>
+      <c r="I29" s="8">
+        <v>2.85E7</v>
+      </c>
+      <c r="J29" s="8">
+        <v>3.6343619E7</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="B30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
+      <c r="C30" s="8">
+        <v>2.1E7</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1.5512418E7</v>
+      </c>
+      <c r="E30" s="8">
+        <v>9692046.0</v>
+      </c>
+      <c r="F30" s="8">
+        <v>6895746.0</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4895746.0</v>
+      </c>
+      <c r="H30" s="8">
+        <v>-2156381.0</v>
+      </c>
+      <c r="I30" s="8">
+        <v>2.6343619E7</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2.6343619E7</v>
+      </c>
+    </row>
     <row r="31" ht="14.25" customHeight="1"/>
     <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>